<commit_message>
produce plots for presentation
</commit_message>
<xml_diff>
--- a/test_data2/issvd_cols.xlsx
+++ b/test_data2/issvd_cols.xlsx
@@ -451,16 +451,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -479,30 +479,30 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -521,30 +521,30 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -591,16 +591,16 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -619,27 +619,27 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
@@ -653,10 +653,10 @@
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -675,27 +675,27 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
@@ -703,16 +703,16 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -731,41 +731,41 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -787,13 +787,13 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
@@ -871,30 +871,30 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -913,13 +913,13 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D35" t="n">
         <v>0</v>
@@ -955,13 +955,13 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" t="n">
         <v>0</v>
@@ -969,16 +969,16 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -1031,21 +1031,21 @@
         <v>0</v>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D44" t="n">
         <v>0</v>
@@ -1067,27 +1067,27 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47" t="n">
         <v>0</v>
@@ -1129,10 +1129,10 @@
         <v>0</v>
       </c>
       <c r="C50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
@@ -1151,41 +1151,41 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C52" t="n">
         <v>0</v>
       </c>
       <c r="D52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C53" t="n">
         <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D54" t="n">
         <v>0</v>
@@ -1193,16 +1193,16 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C55" t="n">
         <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1249,16 +1249,16 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C59" t="n">
         <v>0</v>
       </c>
       <c r="D59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
@@ -1269,10 +1269,10 @@
         <v>0</v>
       </c>
       <c r="C60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -1283,24 +1283,24 @@
         <v>0</v>
       </c>
       <c r="C61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C62" t="n">
         <v>0</v>
       </c>
       <c r="D62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63">
@@ -1333,13 +1333,13 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D65" t="n">
         <v>0</v>
@@ -1347,13 +1347,13 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D66" t="n">
         <v>0</v>
@@ -1381,24 +1381,24 @@
         <v>0</v>
       </c>
       <c r="C68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C69" t="n">
         <v>0</v>
       </c>
       <c r="D69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70">
@@ -1431,13 +1431,13 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C72" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D72" t="n">
         <v>0</v>
@@ -1459,13 +1459,13 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C74" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D74" t="n">
         <v>0</v>
@@ -1473,16 +1473,16 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C75" t="n">
         <v>0</v>
       </c>
       <c r="D75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -1493,24 +1493,24 @@
         <v>0</v>
       </c>
       <c r="C76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B77" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C77" t="n">
         <v>0</v>
       </c>
       <c r="D77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
@@ -1543,30 +1543,30 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C80" t="n">
         <v>0</v>
       </c>
       <c r="D80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C81" t="n">
         <v>0</v>
       </c>
       <c r="D81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -1585,13 +1585,13 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C83" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D83" t="n">
         <v>0</v>
@@ -1627,16 +1627,16 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B86" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C86" t="n">
         <v>0</v>
       </c>
       <c r="D86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87">
@@ -1683,16 +1683,16 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C90" t="n">
         <v>0</v>
       </c>
       <c r="D90" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -1703,10 +1703,10 @@
         <v>0</v>
       </c>
       <c r="C91" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
@@ -1739,13 +1739,13 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B94" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D94" t="n">
         <v>0</v>
@@ -1809,13 +1809,13 @@
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C99" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D99" t="n">
         <v>0</v>
@@ -1837,16 +1837,16 @@
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B101" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C101" t="n">
         <v>0</v>
       </c>
       <c r="D101" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1884,27 +1884,27 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -1912,27 +1912,27 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -1968,13 +1968,13 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -1982,16 +1982,16 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -2010,13 +2010,13 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
@@ -2038,41 +2038,41 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
@@ -2086,10 +2086,10 @@
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -2100,10 +2100,10 @@
         <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -2114,21 +2114,21 @@
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
@@ -2136,13 +2136,13 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
@@ -2164,13 +2164,13 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
@@ -2178,16 +2178,16 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -2206,55 +2206,55 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28" t="n">
         <v>0</v>
@@ -2276,13 +2276,13 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" t="n">
         <v>0</v>
@@ -2304,30 +2304,30 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -2346,16 +2346,16 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -2380,10 +2380,10 @@
         <v>0</v>
       </c>
       <c r="C37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -2394,10 +2394,10 @@
         <v>0</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -2416,16 +2416,16 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -2464,52 +2464,52 @@
         <v>0</v>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -2528,58 +2528,58 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2617,13 +2617,13 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -2673,27 +2673,27 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -2729,16 +2729,16 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -2757,55 +2757,55 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
@@ -2827,27 +2827,27 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
@@ -2875,24 +2875,24 @@
         <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -2911,13 +2911,13 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
@@ -2925,30 +2925,30 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -2981,13 +2981,13 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" t="n">
         <v>0</v>
@@ -3009,13 +3009,13 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" t="n">
         <v>0</v>
@@ -3023,16 +3023,16 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -3071,10 +3071,10 @@
         <v>0</v>
       </c>
       <c r="C34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -3135,16 +3135,16 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
@@ -3155,24 +3155,24 @@
         <v>0</v>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -3205,41 +3205,41 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46" t="n">
         <v>0</v>
@@ -3261,13 +3261,13 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48" t="n">
         <v>0</v>
@@ -3275,27 +3275,27 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50" t="n">
         <v>0</v>
@@ -3317,41 +3317,41 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C52" t="n">
         <v>0</v>
       </c>
       <c r="D52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D54" t="n">
         <v>0</v>
@@ -3387,13 +3387,13 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D57" t="n">
         <v>0</v>
@@ -3407,10 +3407,10 @@
         <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -3443,16 +3443,16 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C61" t="n">
         <v>0</v>
       </c>
       <c r="D61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62">
@@ -3499,13 +3499,13 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D65" t="n">
         <v>0</v>
@@ -3527,13 +3527,13 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D67" t="n">
         <v>0</v>
@@ -3547,10 +3547,10 @@
         <v>0</v>
       </c>
       <c r="C68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69">
@@ -3561,10 +3561,10 @@
         <v>0</v>
       </c>
       <c r="C69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -3583,13 +3583,13 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D71" t="n">
         <v>0</v>
@@ -3611,27 +3611,27 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C73" t="n">
         <v>0</v>
       </c>
       <c r="D73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C74" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D74" t="n">
         <v>0</v>
@@ -3653,16 +3653,16 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C76" t="n">
         <v>0</v>
       </c>
       <c r="D76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77">
@@ -3709,30 +3709,30 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C80" t="n">
         <v>0</v>
       </c>
       <c r="D80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C81" t="n">
         <v>0</v>
       </c>
       <c r="D81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82">
@@ -3751,13 +3751,13 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B83" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D83" t="n">
         <v>0</v>
@@ -3779,16 +3779,16 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C85" t="n">
         <v>0</v>
       </c>
       <c r="D85" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -3813,10 +3813,10 @@
         <v>0</v>
       </c>
       <c r="C87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D87" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -3883,52 +3883,52 @@
         <v>0</v>
       </c>
       <c r="C92" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D92" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C93" t="n">
         <v>0</v>
       </c>
       <c r="D93" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C94" t="n">
         <v>0</v>
       </c>
       <c r="D94" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B95" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96">
@@ -3961,16 +3961,16 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B98" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C98" t="n">
         <v>0</v>
       </c>
       <c r="D98" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99">
@@ -3995,10 +3995,10 @@
         <v>0</v>
       </c>
       <c r="C100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D100" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101">
@@ -4031,16 +4031,16 @@
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B103" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C103" t="n">
         <v>0</v>
       </c>
       <c r="D103" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104">
@@ -4059,27 +4059,27 @@
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B105" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C105" t="n">
         <v>0</v>
       </c>
       <c r="D105" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B106" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C106" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D106" t="n">
         <v>0</v>
@@ -4101,16 +4101,16 @@
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B108" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C108" t="n">
         <v>0</v>
       </c>
       <c r="D108" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109">
@@ -4143,13 +4143,13 @@
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B111" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C111" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D111" t="n">
         <v>0</v>
@@ -4157,16 +4157,16 @@
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B112" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C112" t="n">
         <v>0</v>
       </c>
       <c r="D112" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113">
@@ -4185,30 +4185,30 @@
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B114" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C114" t="n">
         <v>0</v>
       </c>
       <c r="D114" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B115" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C115" t="n">
         <v>0</v>
       </c>
       <c r="D115" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116">
@@ -4227,13 +4227,13 @@
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B117" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C117" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D117" t="n">
         <v>0</v>
@@ -4325,13 +4325,13 @@
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B124" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C124" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D124" t="n">
         <v>0</v>
@@ -4353,13 +4353,13 @@
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B126" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C126" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D126" t="n">
         <v>0</v>
@@ -4381,13 +4381,13 @@
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C128" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D128" t="n">
         <v>0</v>
@@ -4395,13 +4395,13 @@
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C129" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D129" t="n">
         <v>0</v>
@@ -4415,10 +4415,10 @@
         <v>0</v>
       </c>
       <c r="C130" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D130" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131">
@@ -4432,7 +4432,7 @@
         <v>1</v>
       </c>
       <c r="D131" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132">
@@ -4457,10 +4457,10 @@
         <v>0</v>
       </c>
       <c r="C133" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D133" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134">
@@ -4471,10 +4471,10 @@
         <v>0</v>
       </c>
       <c r="C134" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D134" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135">
@@ -4493,13 +4493,13 @@
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B136" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D136" t="n">
         <v>0</v>
@@ -4513,21 +4513,21 @@
         <v>0</v>
       </c>
       <c r="C137" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D137" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B138" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C138" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D138" t="n">
         <v>0</v>
@@ -4535,30 +4535,30 @@
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B139" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C139" t="n">
         <v>0</v>
       </c>
       <c r="D139" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B140" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C140" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D140" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141">
@@ -4591,30 +4591,30 @@
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B143" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C143" t="n">
         <v>0</v>
       </c>
       <c r="D143" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B144" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C144" t="n">
         <v>0</v>
       </c>
       <c r="D144" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145">
@@ -4703,44 +4703,44 @@
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B151" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C151" t="n">
         <v>0</v>
       </c>
       <c r="D151" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B152" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C152" t="n">
         <v>0</v>
       </c>
       <c r="D152" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B153" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C153" t="n">
         <v>0</v>
       </c>
       <c r="D153" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154">
@@ -4773,13 +4773,13 @@
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B156" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C156" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D156" t="n">
         <v>0</v>
@@ -4801,16 +4801,16 @@
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B158" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C158" t="n">
         <v>0</v>
       </c>
       <c r="D158" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159">
@@ -4829,27 +4829,27 @@
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B160" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C160" t="n">
         <v>0</v>
       </c>
       <c r="D160" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B161" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C161" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D161" t="n">
         <v>0</v>
@@ -4857,16 +4857,16 @@
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B162" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C162" t="n">
         <v>0</v>
       </c>
       <c r="D162" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163">
@@ -4877,10 +4877,10 @@
         <v>0</v>
       </c>
       <c r="C163" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D163" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164">
@@ -4891,10 +4891,10 @@
         <v>0</v>
       </c>
       <c r="C164" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D164" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165">
@@ -4913,16 +4913,16 @@
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B166" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C166" t="n">
         <v>0</v>
       </c>
       <c r="D166" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167">
@@ -4941,16 +4941,16 @@
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B168" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C168" t="n">
         <v>0</v>
       </c>
       <c r="D168" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169">
@@ -4983,13 +4983,13 @@
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B171" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C171" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D171" t="n">
         <v>0</v>
@@ -4997,44 +4997,44 @@
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B172" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C172" t="n">
         <v>0</v>
       </c>
       <c r="D172" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B173" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C173" t="n">
         <v>0</v>
       </c>
       <c r="D173" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B174" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C174" t="n">
         <v>0</v>
       </c>
       <c r="D174" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175">
@@ -5053,13 +5053,13 @@
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B176" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C176" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D176" t="n">
         <v>0</v>
@@ -5073,10 +5073,10 @@
         <v>0</v>
       </c>
       <c r="C177" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D177" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="178">
@@ -5109,13 +5109,13 @@
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B180" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C180" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D180" t="n">
         <v>0</v>
@@ -5137,44 +5137,44 @@
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B182" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C182" t="n">
         <v>0</v>
       </c>
       <c r="D182" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B183" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C183" t="n">
         <v>0</v>
       </c>
       <c r="D183" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B184" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C184" t="n">
         <v>0</v>
       </c>
       <c r="D184" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="185">
@@ -5185,10 +5185,10 @@
         <v>0</v>
       </c>
       <c r="C185" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D185" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="186">
@@ -5207,16 +5207,16 @@
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B187" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C187" t="n">
         <v>0</v>
       </c>
       <c r="D187" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="188">
@@ -5235,16 +5235,16 @@
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B189" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C189" t="n">
         <v>0</v>
       </c>
       <c r="D189" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190">
@@ -5305,13 +5305,13 @@
     </row>
     <row r="194">
       <c r="A194" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B194" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C194" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D194" t="n">
         <v>0</v>
@@ -5319,16 +5319,16 @@
     </row>
     <row r="195">
       <c r="A195" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B195" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C195" t="n">
         <v>0</v>
       </c>
       <c r="D195" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="196">
@@ -5361,13 +5361,13 @@
     </row>
     <row r="198">
       <c r="A198" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B198" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C198" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D198" t="n">
         <v>0</v>
@@ -5381,21 +5381,21 @@
         <v>0</v>
       </c>
       <c r="C199" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D199" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B200" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C200" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D200" t="n">
         <v>0</v>
@@ -5403,16 +5403,16 @@
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B201" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C201" t="n">
         <v>0</v>
       </c>
       <c r="D201" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="202">
@@ -5445,16 +5445,16 @@
     </row>
     <row r="204">
       <c r="A204" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B204" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C204" t="n">
         <v>0</v>
       </c>
       <c r="D204" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="205">
@@ -5487,83 +5487,83 @@
     </row>
     <row r="207">
       <c r="A207" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B207" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C207" t="n">
         <v>0</v>
       </c>
       <c r="D207" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B208" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C208" t="n">
         <v>0</v>
       </c>
       <c r="D208" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B209" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C209" t="n">
         <v>0</v>
       </c>
       <c r="D209" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B210" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C210" t="n">
         <v>0</v>
       </c>
       <c r="D210" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B211" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C211" t="n">
         <v>0</v>
       </c>
       <c r="D211" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B212" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C212" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D212" t="n">
         <v>0</v>
@@ -5585,16 +5585,16 @@
     </row>
     <row r="214">
       <c r="A214" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B214" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C214" t="n">
         <v>0</v>
       </c>
       <c r="D214" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="215">
@@ -5613,16 +5613,16 @@
     </row>
     <row r="216">
       <c r="A216" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B216" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C216" t="n">
         <v>0</v>
       </c>
       <c r="D216" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="217">
@@ -5633,10 +5633,10 @@
         <v>0</v>
       </c>
       <c r="C217" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D217" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="218">
@@ -5661,52 +5661,52 @@
         <v>0</v>
       </c>
       <c r="C219" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D219" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B220" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C220" t="n">
         <v>0</v>
       </c>
       <c r="D220" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B221" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C221" t="n">
         <v>0</v>
       </c>
       <c r="D221" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B222" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C222" t="n">
         <v>0</v>
       </c>
       <c r="D222" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="223">
@@ -5725,44 +5725,44 @@
     </row>
     <row r="224">
       <c r="A224" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B224" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C224" t="n">
         <v>0</v>
       </c>
       <c r="D224" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B225" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C225" t="n">
         <v>0</v>
       </c>
       <c r="D225" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B226" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C226" t="n">
         <v>0</v>
       </c>
       <c r="D226" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="227">
@@ -5851,16 +5851,16 @@
     </row>
     <row r="233">
       <c r="A233" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B233" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C233" t="n">
         <v>0</v>
       </c>
       <c r="D233" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="234">
@@ -5871,10 +5871,10 @@
         <v>0</v>
       </c>
       <c r="C234" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D234" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="235">
@@ -5893,41 +5893,41 @@
     </row>
     <row r="236">
       <c r="A236" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B236" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C236" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D236" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B237" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C237" t="n">
         <v>0</v>
       </c>
       <c r="D237" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B238" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C238" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D238" t="n">
         <v>0</v>
@@ -5935,44 +5935,44 @@
     </row>
     <row r="239">
       <c r="A239" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B239" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C239" t="n">
         <v>0</v>
       </c>
       <c r="D239" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B240" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C240" t="n">
         <v>0</v>
       </c>
       <c r="D240" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B241" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C241" t="n">
         <v>0</v>
       </c>
       <c r="D241" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="242">
@@ -5991,13 +5991,13 @@
     </row>
     <row r="243">
       <c r="A243" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B243" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C243" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D243" t="n">
         <v>0</v>
@@ -6033,16 +6033,16 @@
     </row>
     <row r="246">
       <c r="A246" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B246" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C246" t="n">
         <v>0</v>
       </c>
       <c r="D246" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="247">
@@ -6075,13 +6075,13 @@
     </row>
     <row r="249">
       <c r="A249" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B249" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C249" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D249" t="n">
         <v>0</v>
@@ -6089,30 +6089,30 @@
     </row>
     <row r="250">
       <c r="A250" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B250" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C250" t="n">
         <v>0</v>
       </c>
       <c r="D250" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B251" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C251" t="n">
         <v>0</v>
       </c>
       <c r="D251" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>